<commit_message>
Ajustes na ontologia para criar mais uma propriedade. Ajuste no SDD para criar o relation ??questao ontriscal:Questao	ontriscal:fazParte ontriscal:GrupoDeQuestao
</commit_message>
<xml_diff>
--- a/templates de metados semanticos/metadata/SDD-RISKSTRAT-EXP-1-2021.xlsx
+++ b/templates de metados semanticos/metadata/SDD-RISKSTRAT-EXP-1-2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\estratificacaoderiscosaudemental\templates de metados semanticos\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04244A16-87C1-4672-80C2-A567027C67DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DA7C45-8D01-408F-86D8-E0AA7C4796D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="382">
   <si>
     <t>Attribute</t>
   </si>
@@ -1202,6 +1202,12 @@
   </si>
   <si>
     <t>ontriscal:VulnerabilidadeSocial</t>
+  </si>
+  <si>
+    <t>ontriscal:fazParte</t>
+  </si>
+  <si>
+    <t>ontriscal:GrupoDeQuestao</t>
   </si>
 </sst>
 </file>
@@ -3929,11 +3935,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:KK208"/>
+  <dimension ref="A1:KK209"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -17269,20 +17273,20 @@
     </row>
     <row r="65" spans="1:41" ht="15.75" customHeight="1">
       <c r="A65" s="29" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B65" s="29"/>
       <c r="C65" s="29"/>
       <c r="D65" s="29" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E65" s="29"/>
       <c r="F65" s="29"/>
       <c r="G65" s="29" t="s">
-        <v>358</v>
+        <v>380</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>355</v>
+        <v>381</v>
       </c>
       <c r="I65" s="29"/>
       <c r="J65" s="29"/>
@@ -17320,17 +17324,21 @@
     </row>
     <row r="66" spans="1:41" ht="15.75" customHeight="1">
       <c r="A66" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B66" s="29"/>
       <c r="C66" s="29"/>
       <c r="D66" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E66" s="29"/>
       <c r="F66" s="29"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="29"/>
+      <c r="G66" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="H66" s="29" t="s">
+        <v>355</v>
+      </c>
       <c r="I66" s="29"/>
       <c r="J66" s="29"/>
       <c r="K66" s="29"/>
@@ -17367,12 +17375,12 @@
     </row>
     <row r="67" spans="1:41" ht="15.75" customHeight="1">
       <c r="A67" s="29" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B67" s="29"/>
       <c r="C67" s="29"/>
       <c r="D67" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E67" s="29"/>
       <c r="F67" s="29"/>
@@ -17414,21 +17422,17 @@
     </row>
     <row r="68" spans="1:41" ht="15.75" customHeight="1">
       <c r="A68" s="29" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B68" s="29"/>
       <c r="C68" s="29"/>
       <c r="D68" s="29" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="E68" s="29"/>
       <c r="F68" s="29"/>
-      <c r="G68" s="29" t="s">
-        <v>361</v>
-      </c>
-      <c r="H68" s="29" t="s">
-        <v>359</v>
-      </c>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
       <c r="I68" s="29"/>
       <c r="J68" s="29"/>
       <c r="K68" s="29"/>
@@ -17478,7 +17482,7 @@
         <v>361</v>
       </c>
       <c r="H69" s="29" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="I69" s="29"/>
       <c r="J69" s="29"/>
@@ -17529,7 +17533,7 @@
         <v>361</v>
       </c>
       <c r="H70" s="29" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="I70" s="29"/>
       <c r="J70" s="29"/>
@@ -17567,20 +17571,20 @@
     </row>
     <row r="71" spans="1:41" ht="15.75" customHeight="1">
       <c r="A71" s="29" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B71" s="29"/>
       <c r="C71" s="29"/>
       <c r="D71" s="29" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E71" s="29"/>
       <c r="F71" s="29"/>
       <c r="G71" s="29" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H71" s="29" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="I71" s="29"/>
       <c r="J71" s="29"/>
@@ -17618,20 +17622,20 @@
     </row>
     <row r="72" spans="1:41" ht="15.75" customHeight="1">
       <c r="A72" s="29" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B72" s="29"/>
       <c r="C72" s="29"/>
       <c r="D72" s="29" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="E72" s="29"/>
       <c r="F72" s="29"/>
       <c r="G72" s="29" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="H72" s="29" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="I72" s="29"/>
       <c r="J72" s="29"/>
@@ -17669,20 +17673,20 @@
     </row>
     <row r="73" spans="1:41" ht="15.75" customHeight="1">
       <c r="A73" s="29" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="B73" s="29"/>
       <c r="C73" s="29"/>
       <c r="D73" s="29" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="E73" s="29"/>
       <c r="F73" s="29"/>
       <c r="G73" s="29" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="I73" s="29"/>
       <c r="J73" s="29"/>
@@ -17720,20 +17724,20 @@
     </row>
     <row r="74" spans="1:41" ht="15.75" customHeight="1">
       <c r="A74" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B74" s="29"/>
       <c r="C74" s="29"/>
       <c r="D74" s="29" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="E74" s="29"/>
       <c r="F74" s="29"/>
       <c r="G74" s="29" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I74" s="29"/>
       <c r="J74" s="29"/>
@@ -17771,20 +17775,20 @@
     </row>
     <row r="75" spans="1:41" ht="15.75" customHeight="1">
       <c r="A75" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B75" s="29"/>
       <c r="C75" s="29"/>
       <c r="D75" s="29" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E75" s="29"/>
       <c r="F75" s="29"/>
       <c r="G75" s="29" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="H75" s="29" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I75" s="29"/>
       <c r="J75" s="29"/>
@@ -17835,7 +17839,7 @@
         <v>364</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I76" s="29"/>
       <c r="J76" s="29"/>
@@ -17886,7 +17890,7 @@
         <v>364</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I77" s="29"/>
       <c r="J77" s="29"/>
@@ -17924,12 +17928,12 @@
     </row>
     <row r="78" spans="1:41" ht="15.75" customHeight="1">
       <c r="A78" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B78" s="29"/>
       <c r="C78" s="29"/>
       <c r="D78" s="29" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E78" s="29"/>
       <c r="F78" s="29"/>
@@ -17937,7 +17941,7 @@
         <v>364</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="I78" s="29"/>
       <c r="J78" s="29"/>
@@ -17988,7 +17992,7 @@
         <v>364</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I79" s="29"/>
       <c r="J79" s="29"/>
@@ -18039,7 +18043,7 @@
         <v>364</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I80" s="29"/>
       <c r="J80" s="29"/>
@@ -18077,12 +18081,12 @@
     </row>
     <row r="81" spans="1:41" ht="15.75" customHeight="1">
       <c r="A81" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B81" s="29"/>
       <c r="C81" s="29"/>
       <c r="D81" s="29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E81" s="29"/>
       <c r="F81" s="29"/>
@@ -18090,7 +18094,7 @@
         <v>364</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="I81" s="29"/>
       <c r="J81" s="29"/>
@@ -18141,7 +18145,7 @@
         <v>364</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I82" s="29"/>
       <c r="J82" s="29"/>
@@ -18192,7 +18196,7 @@
         <v>364</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I83" s="29"/>
       <c r="J83" s="29"/>
@@ -18230,20 +18234,20 @@
     </row>
     <row r="84" spans="1:41" ht="15.75" customHeight="1">
       <c r="A84" s="29" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="B84" s="29"/>
       <c r="C84" s="29"/>
       <c r="D84" s="29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E84" s="29"/>
       <c r="F84" s="29"/>
       <c r="G84" s="29" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="H84" s="29" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="I84" s="29"/>
       <c r="J84" s="29"/>
@@ -18281,12 +18285,12 @@
     </row>
     <row r="85" spans="1:41" ht="15.75" customHeight="1">
       <c r="A85" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B85" s="29"/>
       <c r="C85" s="29"/>
       <c r="D85" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E85" s="29"/>
       <c r="F85" s="29"/>
@@ -18332,12 +18336,12 @@
     </row>
     <row r="86" spans="1:41" ht="15.75" customHeight="1">
       <c r="A86" s="29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B86" s="29"/>
       <c r="C86" s="29"/>
       <c r="D86" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E86" s="29"/>
       <c r="F86" s="29"/>
@@ -18383,12 +18387,12 @@
     </row>
     <row r="87" spans="1:41" ht="15.75" customHeight="1">
       <c r="A87" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B87" s="29"/>
       <c r="C87" s="29"/>
       <c r="D87" s="29" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E87" s="29"/>
       <c r="F87" s="29"/>
@@ -18433,14 +18437,22 @@
       <c r="AO87" s="29"/>
     </row>
     <row r="88" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A88" s="29"/>
+      <c r="A88" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="B88" s="29"/>
       <c r="C88" s="29"/>
-      <c r="D88" s="29"/>
+      <c r="D88" s="29" t="s">
+        <v>379</v>
+      </c>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
-      <c r="G88" s="29"/>
-      <c r="H88" s="29"/>
+      <c r="G88" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="H88" s="29" t="s">
+        <v>376</v>
+      </c>
       <c r="I88" s="29"/>
       <c r="J88" s="29"/>
       <c r="K88" s="29"/>
@@ -23635,6 +23647,49 @@
       <c r="AN208" s="29"/>
       <c r="AO208" s="29"/>
     </row>
+    <row r="209" spans="1:41" ht="15.75" customHeight="1">
+      <c r="A209" s="29"/>
+      <c r="B209" s="29"/>
+      <c r="C209" s="29"/>
+      <c r="D209" s="29"/>
+      <c r="E209" s="29"/>
+      <c r="F209" s="29"/>
+      <c r="G209" s="29"/>
+      <c r="H209" s="29"/>
+      <c r="I209" s="29"/>
+      <c r="J209" s="29"/>
+      <c r="K209" s="29"/>
+      <c r="L209" s="29"/>
+      <c r="M209" s="29"/>
+      <c r="N209" s="29"/>
+      <c r="O209" s="29"/>
+      <c r="P209" s="29"/>
+      <c r="Q209" s="29"/>
+      <c r="R209" s="29"/>
+      <c r="S209" s="29"/>
+      <c r="T209" s="29"/>
+      <c r="U209" s="29"/>
+      <c r="V209" s="29"/>
+      <c r="W209" s="29"/>
+      <c r="X209" s="29"/>
+      <c r="Y209" s="29"/>
+      <c r="Z209" s="29"/>
+      <c r="AA209" s="29"/>
+      <c r="AB209" s="29"/>
+      <c r="AC209" s="29"/>
+      <c r="AD209" s="29"/>
+      <c r="AE209" s="29"/>
+      <c r="AF209" s="29"/>
+      <c r="AG209" s="29"/>
+      <c r="AH209" s="29"/>
+      <c r="AI209" s="29"/>
+      <c r="AJ209" s="29"/>
+      <c r="AK209" s="29"/>
+      <c r="AL209" s="29"/>
+      <c r="AM209" s="29"/>
+      <c r="AN209" s="29"/>
+      <c r="AO209" s="29"/>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atores participantes da mudança: Evaldo de Oliveira da Silva Questão de competência respondida: Naõ se aplica. Data/Hora da mudança. 10 de Março de 2022. 16h26 Coleção de dados anotada. DA-RISKSTRAT-2021-A.csv Descrição da mudança. Alteração do codebook para inserir os códigos e a ontologia Ontriscal. Solicitação do Professor Paulo.
</commit_message>
<xml_diff>
--- a/templates de metados semanticos/metadata/SDD-RISKSTRAT-EXP-1-2021.xlsx
+++ b/templates de metados semanticos/metadata/SDD-RISKSTRAT-EXP-1-2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\estratificacaoderiscosaudemental\templates de metados semanticos\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DA7C45-8D01-408F-86D8-E0AA7C4796D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8923D19-C0A8-4E12-A86D-15DEA751C29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="384">
   <si>
     <t>Attribute</t>
   </si>
@@ -1208,6 +1208,12 @@
   </si>
   <si>
     <t>ontriscal:GrupoDeQuestao</t>
+  </si>
+  <si>
+    <t>TipodeComorbidadeououtracondicaocronicaclinicaassociada</t>
+  </si>
+  <si>
+    <t>Grupo6_4_Comorbidadeououtracondicaocronicaclinicaassociada?</t>
   </si>
 </sst>
 </file>
@@ -3937,7 +3943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:KK209"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -14421,7 +14429,7 @@
     </row>
     <row r="35" spans="1:297" ht="13.7" customHeight="1">
       <c r="A35" s="29" t="s">
-        <v>336</v>
+        <v>383</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>346</v>
@@ -14728,7 +14736,7 @@
     </row>
     <row r="36" spans="1:297" ht="13.7" customHeight="1">
       <c r="A36" s="29" t="s">
-        <v>337</v>
+        <v>382</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>350</v>

</xml_diff>